<commit_message>
update fonts to helvetica
</commit_message>
<xml_diff>
--- a/assets/intro/Chetty-graph.xlsx
+++ b/assets/intro/Chetty-graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jim\Documents\GitHub\book\assets\intro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F135A695-1941-4EA7-A149-90E401CF52D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5256608-AA86-4800-AA4C-731008E5B152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F7506CF1-42A2-0E40-ACF3-CE4CBEA862E1}"/>
   </bookViews>
@@ -70,13 +70,11 @@
       <sz val="12"/>
       <color rgb="FF24292E"/>
       <name val="Helvetica"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF24292E"/>
+      <color theme="1"/>
       <name val="Helvetica"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,7 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,12 +500,9 @@
             <a:pPr>
               <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -553,10 +548,7 @@
                 <a:pPr>
                   <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -564,12 +556,25 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1600" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+                  </a:rPr>
                   <a:t>Percent of studies</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="5.5366966840704253E-2"/>
+              <c:y val="0.30844042655157539"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -585,10 +590,7 @@
               <a:pPr>
                 <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -617,12 +619,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -669,12 +668,9 @@
           <a:pPr>
             <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -722,7 +718,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1623,13 +1619,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC2AB39-02F0-1040-BABD-08B2E2892E08}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="11" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1647,138 +1646,139 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1979</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>50</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1979</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>29</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>1979</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>13</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>1979</v>
       </c>
       <c r="H3" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>1990</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>38</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>1990</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>33</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>1990</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>17</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>1990</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>2000</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>65</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>2000</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>56</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>2000</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>48</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>2000</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>2010</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>75</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>2010</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>60</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>2010</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>69</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>2010</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>